<commit_message>
update with more resources
</commit_message>
<xml_diff>
--- a/CodeSystem-hn-appointment-flag-code-cs.xlsx
+++ b/CodeSystem-hn-appointment-flag-code-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-25T11:50:22+02:00</t>
+    <t>2023-09-25T15:31:18+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
   </si>
   <si>
     <t>Level</t>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Innbygger kan be om endret time</t>
+  </si>
+  <si>
+    <t>canHaveAppointmentDetails</t>
+  </si>
+  <si>
+    <t>Det finnes ytterlege timedetaljer på time/timeavtale som kan hentes</t>
+  </si>
+  <si>
+    <t>canInitateDialog</t>
+  </si>
+  <si>
+    <t>Dialog kan inisieres</t>
   </si>
 </sst>
 </file>
@@ -469,7 +481,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -573,6 +585,30 @@
       </c>
       <c r="D8" s="2"/>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
update with minor changes and new example
</commit_message>
<xml_diff>
--- a/CodeSystem-hn-appointment-flag-code-cs.xlsx
+++ b/CodeSystem-hn-appointment-flag-code-cs.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-08T01:12:56+01:00</t>
+    <t>2023-11-08T15:53:02+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -183,7 +183,7 @@
     <t>Det finnes ytterlege timedetaljer på time/timeavtale som kan hentes</t>
   </si>
   <si>
-    <t>canInitateDialog</t>
+    <t>canInitiateDialog</t>
   </si>
   <si>
     <t>Dialog kan inisieres</t>

</xml_diff>